<commit_message>
ITPM Excel template New changes
</commit_message>
<xml_diff>
--- a/ITPM - Import Excel Template/MEGA_USR/ITPM Template v4.xlsx
+++ b/ITPM - Import Excel Template/MEGA_USR/ITPM Template v4.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MAM\Desktop\ITPM TEMPLATE EXCEL IMPORT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MAM\Desktop\ITPM - Import Excel Template\MEGA_USR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40269138-D16A-4EA7-874B-B469D8C8CC1A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F61D862-26C2-4E1F-9849-9612FC65286B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="961" firstSheet="6" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="961" firstSheet="6" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="_README" sheetId="18" r:id="rId1"/>
@@ -69,7 +69,35 @@
     <author>AIT MOUSSA Mohamed</author>
   </authors>
   <commentList>
-    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{B2582373-543A-4231-9262-BD036358D9DA}">
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{E00F0B95-EE1D-4F8A-A360-25C86CA3D5CE}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Cloud Computing Value : 
+-On-Premises
+-Cloud: IaaS
+-Cloud: PaaS
+-Cloud: SaaS</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{B2582373-543A-4231-9262-BD036358D9DA}">
       <text>
         <r>
           <rPr>
@@ -89,7 +117,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{D93F7CD3-F570-4FFD-B1C6-AE04EFA94A4A}">
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{D93F7CD3-F570-4FFD-B1C6-AE04EFA94A4A}">
       <text>
         <r>
           <rPr>
@@ -244,6 +272,23 @@
           </rPr>
           <t xml:space="preserve">
 </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{B1A1CC1B-117A-4358-B125-F45D189631B4}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>State Values : 
+-Production
+-Preparation
+-Retirement</t>
         </r>
       </text>
     </comment>
@@ -573,7 +618,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="234">
   <si>
     <t>Software Technology</t>
   </si>
@@ -614,9 +659,6 @@
     <t>E9E1009852444403</t>
   </si>
   <si>
-    <t>A1A5A2B352D70CF1</t>
-  </si>
-  <si>
     <t>A1A5A23D52D70C28</t>
   </si>
   <si>
@@ -785,9 +827,6 @@
     <t>87298DEA4FA34A8D</t>
   </si>
   <si>
-    <t>2AA34A164FAA027E</t>
-  </si>
-  <si>
     <t>87298DF54FA34AA2</t>
   </si>
   <si>
@@ -939,12 +978,6 @@
   </si>
   <si>
     <t>55BD75C0512356A0</t>
-  </si>
-  <si>
-    <t>DA5D19D34F7B5959</t>
-  </si>
-  <si>
-    <t>DA5D19C54F7B593F</t>
   </si>
   <si>
     <t>C873D0D35E1E4B04</t>
@@ -1284,11 +1317,32 @@
   <si>
     <t>6112E0415E7C0166</t>
   </si>
+  <si>
+    <t>Cloud Computing</t>
+  </si>
+  <si>
+    <t>=D1:D636Cloud Computing</t>
+  </si>
+  <si>
+    <t>A6F59BA55EA97E29</t>
+  </si>
+  <si>
+    <t>A6F5ED675EA9859D</t>
+  </si>
+  <si>
+    <t>809C94B05E1C5717</t>
+  </si>
+  <si>
+    <t>809C94A65E1C56CA</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="yyyy/m/d;@"/>
+  </numFmts>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -1398,7 +1452,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1423,9 +1477,6 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1457,13 +1508,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="11" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="11" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1473,6 +1518,24 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1879,52 +1942,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:4" s="10" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="B2" s="11" t="s">
-        <v>155</v>
-      </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="13"/>
+    <row r="2" spans="1:4" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="B2" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="C2" s="11"/>
+      <c r="D2" s="12"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D3" s="3"/>
     </row>
     <row r="4" spans="1:4" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="C4" s="14" t="s">
-        <v>157</v>
+        <v>152</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>153</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="4"/>
-      <c r="C5" s="14" t="s">
-        <v>158</v>
+      <c r="C5" s="13" t="s">
+        <v>154</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="4"/>
-      <c r="C6" s="14" t="s">
-        <v>30</v>
+      <c r="C6" s="13" t="s">
+        <v>29</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="26.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="4"/>
-      <c r="C7" s="14" t="s">
-        <v>159</v>
+      <c r="C7" s="13" t="s">
+        <v>155</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1932,29 +1995,29 @@
     </row>
     <row r="9" spans="1:4" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
-        <v>190</v>
-      </c>
-      <c r="C9" s="14" t="s">
-        <v>172</v>
+        <v>186</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>168</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C10" s="14" t="s">
-        <v>160</v>
+      <c r="C10" s="13" t="s">
+        <v>156</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="41.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C11" s="14" t="s">
-        <v>108</v>
+      <c r="C11" s="13" t="s">
+        <v>106</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -1962,77 +2025,77 @@
     </row>
     <row r="13" spans="1:4" ht="65.400000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="C13" s="14" t="s">
+        <v>157</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>187</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C14" s="13" t="s">
+        <v>188</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C15" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C16" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="17" spans="3:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C17" s="13" t="s">
+        <v>205</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="18" spans="3:4" ht="43.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C18" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="19" spans="3:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C19" s="13" t="s">
+        <v>189</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="20" spans="3:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C20" s="13" t="s">
+        <v>206</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="21" spans="3:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C21" s="13" t="s">
+        <v>207</v>
+      </c>
+      <c r="D21" s="3" t="s">
         <v>191</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C14" s="14" t="s">
-        <v>192</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C15" s="14" t="s">
-        <v>162</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C16" s="14" t="s">
-        <v>208</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="17" spans="3:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C17" s="14" t="s">
-        <v>209</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="18" spans="3:4" ht="43.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C18" s="14" t="s">
-        <v>163</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="19" spans="3:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C19" s="14" t="s">
-        <v>193</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="20" spans="3:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C20" s="14" t="s">
-        <v>210</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="21" spans="3:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C21" s="14" t="s">
-        <v>211</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>195</v>
       </c>
     </row>
   </sheetData>
@@ -2047,7 +2110,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q12"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" zoomScale="102" zoomScaleNormal="102" workbookViewId="0">
+    <sheetView zoomScale="102" zoomScaleNormal="102" workbookViewId="0">
       <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
@@ -2056,11 +2119,14 @@
     <col min="1" max="1" width="30.6640625" style="7"/>
     <col min="2" max="4" width="30.6640625" style="2"/>
     <col min="5" max="5" width="27.33203125" style="2" customWidth="1"/>
-    <col min="6" max="17" width="30.6640625" style="2"/>
+    <col min="6" max="6" width="30.6640625" style="25"/>
+    <col min="7" max="9" width="30.6640625" style="2"/>
+    <col min="10" max="15" width="30.6640625" style="25"/>
+    <col min="16" max="17" width="30.6640625" style="2"/>
     <col min="18" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" s="5" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -2074,9 +2140,9 @@
         <v>3</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>223</v>
-      </c>
-      <c r="F1" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="F1" s="26" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="5" t="s">
@@ -2088,23 +2154,23 @@
       <c r="I1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="K1" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="L1" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="M1" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="N1" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="N1" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="O1" s="5" t="s">
-        <v>120</v>
+      <c r="O1" s="26" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="2" spans="1:17" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -2121,37 +2187,37 @@
         <v>11</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>13</v>
+        <v>105</v>
+      </c>
+      <c r="F2" s="27" t="s">
+        <v>231</v>
       </c>
       <c r="G2" s="6" t="s">
         <v>12</v>
       </c>
       <c r="H2" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="J2" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="K2" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="L2" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="M2" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="M2" s="6" t="s">
+      <c r="N2" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="N2" s="6" t="s">
+      <c r="O2" s="27" t="s">
         <v>20</v>
-      </c>
-      <c r="O2" s="6" t="s">
-        <v>21</v>
       </c>
       <c r="P2" s="6"/>
       <c r="Q2" s="6"/>
@@ -2212,10 +2278,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:N6"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+    <sheetView topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="N1" sqref="N1:N1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2224,122 +2290,120 @@
     <col min="2" max="2" width="30.6640625" style="2"/>
     <col min="3" max="3" width="30.77734375" style="2" customWidth="1"/>
     <col min="4" max="4" width="26.21875" style="2" customWidth="1"/>
-    <col min="5" max="12" width="30.6640625" style="2"/>
+    <col min="5" max="9" width="30.6640625" style="2"/>
+    <col min="10" max="10" width="30.6640625" style="25"/>
+    <col min="11" max="12" width="30.6640625" style="2"/>
     <col min="13" max="13" width="18.44140625" style="2" customWidth="1"/>
-    <col min="14" max="14" width="18" style="2" customWidth="1"/>
+    <col min="14" max="14" width="18" style="25" customWidth="1"/>
     <col min="15" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="J1" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="M1" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="N1" s="26" t="s">
         <v>175</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>189</v>
-      </c>
-      <c r="M1" s="5" t="s">
-        <v>178</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="2" spans="1:14" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>9</v>
       </c>
       <c r="C2" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="J2" s="27" t="s">
+        <v>230</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="M2" s="6" t="s">
         <v>176</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="N2" s="27" t="s">
         <v>177</v>
       </c>
-      <c r="E2" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="M2" s="6" t="s">
-        <v>180</v>
-      </c>
-      <c r="N2" s="6" t="s">
-        <v>181</v>
-      </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="J3" s="8"/>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
+      <c r="N3" s="28"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
-      <c r="N4" s="3"/>
+      <c r="N4" s="28"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="L5" s="3"/>
       <c r="M5" s="3"/>
-      <c r="N5" s="9"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="N6" s="8"/>
+      <c r="N5" s="28"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <dataValidations count="5">
+  <dataValidations count="6">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error" error="You must select one of the values available in the drop-down list box" sqref="E3:E501" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>"Capital Expense,Operating Expense,#reset"</formula1>
     </dataValidation>
@@ -2355,6 +2419,9 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3" xr:uid="{4F30D244-9F19-4672-8025-EC095430166C}">
       <formula1>"Application,Software Technology,Server (deployed),#reset"</formula1>
     </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:G1139" xr:uid="{7BD9E8B1-325F-44AB-AB3E-632156ABDAAB}">
+      <formula1>"Production,Preparation,Retirement"</formula1>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2364,10 +2431,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:Q12"/>
+  <dimension ref="A1:Q3"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2376,8 +2443,8 @@
     <col min="2" max="5" width="30.6640625" style="2"/>
     <col min="6" max="6" width="20.6640625" style="2" customWidth="1"/>
     <col min="7" max="7" width="26.109375" style="2" customWidth="1"/>
-    <col min="8" max="12" width="30.6640625" style="2"/>
-    <col min="13" max="13" width="27.88671875" style="2" customWidth="1"/>
+    <col min="8" max="12" width="30.6640625" style="25"/>
+    <col min="13" max="13" width="27.88671875" style="25" customWidth="1"/>
     <col min="14" max="14" width="17.109375" style="2" customWidth="1"/>
     <col min="15" max="15" width="18.77734375" style="2" customWidth="1"/>
     <col min="16" max="16" width="20.109375" style="2" customWidth="1"/>
@@ -2388,7 +2455,7 @@
   <sheetData>
     <row r="1" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>1</v>
@@ -2397,121 +2464,83 @@
         <v>2</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>166</v>
-      </c>
-      <c r="H1" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="H1" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="L1" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="L1" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="M1" s="5" t="s">
-        <v>182</v>
+      <c r="M1" s="26" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="2" spans="1:17" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="B2" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2" s="14" t="s">
         <v>9</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>10</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>215</v>
-      </c>
-      <c r="H2" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="H2" s="27" t="s">
+        <v>128</v>
+      </c>
+      <c r="I2" s="27" t="s">
+        <v>129</v>
+      </c>
+      <c r="J2" s="27" t="s">
+        <v>130</v>
+      </c>
+      <c r="K2" s="27" t="s">
+        <v>131</v>
+      </c>
+      <c r="L2" s="27" t="s">
         <v>132</v>
       </c>
-      <c r="I2" s="22" t="s">
+      <c r="M2" s="27" t="s">
         <v>133</v>
       </c>
-      <c r="J2" s="22" t="s">
-        <v>134</v>
-      </c>
-      <c r="K2" s="22" t="s">
-        <v>135</v>
-      </c>
-      <c r="L2" s="22" t="s">
-        <v>136</v>
-      </c>
-      <c r="M2" s="22" t="s">
-        <v>137</v>
-      </c>
-      <c r="N2" s="23"/>
-      <c r="O2" s="24"/>
-      <c r="P2" s="24"/>
-      <c r="Q2" s="24"/>
+      <c r="N2" s="20"/>
+      <c r="O2" s="21"/>
+      <c r="P2" s="21"/>
+      <c r="Q2" s="21"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="G3" s="3"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="J4" s="8"/>
-      <c r="K4" s="8"/>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="J5" s="8"/>
-      <c r="K5" s="8"/>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="J6" s="8"/>
-      <c r="K6" s="8"/>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="J7" s="8"/>
-      <c r="K7" s="8"/>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="J10" s="8"/>
-      <c r="K10" s="8"/>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="J11" s="8"/>
-      <c r="K11" s="8"/>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="J12" s="8"/>
-      <c r="K12" s="8"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -2528,22 +2557,23 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="I38" sqref="I38"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1:L1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.6640625" style="7"/>
-    <col min="2" max="12" width="30.6640625" style="2"/>
+    <col min="2" max="7" width="30.6640625" style="2"/>
+    <col min="8" max="12" width="30.6640625" style="25"/>
     <col min="13" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>1</v>
@@ -2552,110 +2582,70 @@
         <v>2</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="F1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="K1" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>120</v>
+      <c r="L1" s="26" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="2" spans="1:12" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="B2" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" s="14" t="s">
         <v>9</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>10</v>
       </c>
       <c r="D2" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="F2" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="G2" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="H2" s="27" t="s">
         <v>85</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="I2" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="J2" s="27" t="s">
         <v>87</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="K2" s="27" t="s">
         <v>88</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="L2" s="27" t="s">
         <v>89</v>
       </c>
-      <c r="K2" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="I10" s="8"/>
-      <c r="J10" s="8"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="I11" s="8"/>
-      <c r="J11" s="8"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="I12" s="8"/>
-      <c r="J12" s="8"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -2668,7 +2658,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E2E619E-351A-46F5-A00C-931865AB6684}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
@@ -2684,42 +2674,42 @@
   <sheetData>
     <row r="1" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D1" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="F1" s="5" t="s">
         <v>104</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>164</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>222</v>
+      </c>
+      <c r="B2" t="s">
+        <v>223</v>
+      </c>
+      <c r="C2" t="s">
+        <v>224</v>
+      </c>
+      <c r="D2" t="s">
+        <v>225</v>
+      </c>
+      <c r="E2" t="s">
         <v>226</v>
       </c>
-      <c r="B2" t="s">
+      <c r="F2" s="22" t="s">
         <v>227</v>
-      </c>
-      <c r="C2" t="s">
-        <v>228</v>
-      </c>
-      <c r="D2" t="s">
-        <v>229</v>
-      </c>
-      <c r="E2" t="s">
-        <v>230</v>
-      </c>
-      <c r="F2" s="25" t="s">
-        <v>231</v>
       </c>
     </row>
   </sheetData>
@@ -2738,23 +2728,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4616348E-F67E-4F3C-9919-0A0715B394BA}">
   <dimension ref="A1:O4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="K1" activeCellId="4" sqref="G1:G1048576 H1:H1048576 I1:I1048576 J1:J1048576 K1:K1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.77734375" style="17" customWidth="1"/>
+    <col min="1" max="1" width="23.77734375" style="16" customWidth="1"/>
     <col min="2" max="2" width="20.88671875" style="2" customWidth="1"/>
     <col min="3" max="3" width="19.6640625" style="2" customWidth="1"/>
     <col min="4" max="4" width="29.21875" style="2" customWidth="1"/>
     <col min="5" max="5" width="27.33203125" style="2" customWidth="1"/>
     <col min="6" max="6" width="23" style="2" customWidth="1"/>
-    <col min="7" max="7" width="24.33203125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="27.109375" style="2" customWidth="1"/>
-    <col min="9" max="9" width="23.77734375" style="2" customWidth="1"/>
-    <col min="10" max="10" width="21.44140625" style="2" customWidth="1"/>
-    <col min="11" max="11" width="26.6640625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="24.33203125" style="25" customWidth="1"/>
+    <col min="8" max="8" width="27.109375" style="25" customWidth="1"/>
+    <col min="9" max="9" width="23.77734375" style="25" customWidth="1"/>
+    <col min="10" max="10" width="21.44140625" style="25" customWidth="1"/>
+    <col min="11" max="11" width="26.6640625" style="25" customWidth="1"/>
     <col min="12" max="13" width="18.21875" style="2" customWidth="1"/>
     <col min="14" max="15" width="22.6640625" style="2" customWidth="1"/>
     <col min="16" max="16384" width="8.88671875" style="2"/>
@@ -2762,72 +2752,72 @@
   <sheetData>
     <row r="1" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>138</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>142</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="F1" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="J1" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" s="17" customFormat="1" ht="10.199999999999999" hidden="1" x14ac:dyDescent="0.25">
+      <c r="K1" s="26" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" s="16" customFormat="1" ht="10.199999999999999" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>218</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="G2" s="27" t="s">
+        <v>123</v>
+      </c>
+      <c r="H2" s="27" t="s">
+        <v>124</v>
+      </c>
+      <c r="I2" s="27" t="s">
         <v>125</v>
       </c>
-      <c r="B2" s="15" t="s">
-        <v>139</v>
-      </c>
-      <c r="C2" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="15" t="s">
-        <v>222</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="F2" s="6" t="s">
+      <c r="J2" s="27" t="s">
         <v>126</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="K2" s="27" t="s">
         <v>127</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>131</v>
       </c>
       <c r="L2" s="6"/>
       <c r="M2" s="6"/>
@@ -2837,8 +2827,6 @@
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="E3" s="3"/>
       <c r="F3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="J3" s="8"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="E4" s="3"/>
@@ -2861,7 +2849,7 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="H1" activeCellId="1" sqref="I1:I1048576 H1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2872,14 +2860,14 @@
     <col min="5" max="5" width="18.6640625" style="2" customWidth="1"/>
     <col min="6" max="6" width="23.44140625" style="2" customWidth="1"/>
     <col min="7" max="7" width="21.33203125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="17.88671875" style="2" customWidth="1"/>
-    <col min="9" max="9" width="14.77734375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="17.88671875" style="25" customWidth="1"/>
+    <col min="9" max="9" width="14.77734375" style="25" customWidth="1"/>
     <col min="10" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>1</v>
@@ -2888,57 +2876,55 @@
         <v>2</v>
       </c>
       <c r="D1" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G1" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="H1" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="I1" s="26" t="s">
         <v>114</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="6" customFormat="1" ht="10.199999999999999" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="G2" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="B2" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>218</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>219</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>122</v>
+      <c r="H2" s="27" t="s">
+        <v>233</v>
+      </c>
+      <c r="I2" s="27" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F3" s="3"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F4" s="3"/>
@@ -2978,23 +2964,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{054DD31E-EE39-4F1E-91F5-CA20AA5F6A1D}">
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="K1" activeCellId="6" sqref="F8 F1:F1048576 G1:G1048576 H1:H1048576 I1:I1048576 J1:J1048576 K1:K1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.6640625" style="15" customWidth="1"/>
+    <col min="1" max="1" width="23.6640625" style="14" customWidth="1"/>
     <col min="2" max="2" width="15.33203125" style="2" customWidth="1"/>
     <col min="3" max="3" width="23.88671875" style="2" customWidth="1"/>
     <col min="4" max="4" width="18.88671875" style="2" customWidth="1"/>
     <col min="5" max="5" width="18" style="2" customWidth="1"/>
-    <col min="6" max="6" width="26" style="2" customWidth="1"/>
-    <col min="7" max="7" width="23.6640625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="27.109375" style="2" customWidth="1"/>
-    <col min="9" max="9" width="27" style="2" customWidth="1"/>
-    <col min="10" max="10" width="24.5546875" style="2" customWidth="1"/>
-    <col min="11" max="11" width="22.77734375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="26" style="25" customWidth="1"/>
+    <col min="7" max="7" width="23.6640625" style="25" customWidth="1"/>
+    <col min="8" max="8" width="27.109375" style="25" customWidth="1"/>
+    <col min="9" max="9" width="27" style="25" customWidth="1"/>
+    <col min="10" max="10" width="24.5546875" style="25" customWidth="1"/>
+    <col min="11" max="11" width="22.77734375" style="25" customWidth="1"/>
     <col min="12" max="12" width="22.5546875" style="2" customWidth="1"/>
     <col min="13" max="13" width="19.21875" style="2" customWidth="1"/>
     <col min="14" max="14" width="28" style="2" customWidth="1"/>
@@ -3004,72 +2990,72 @@
   <sheetData>
     <row r="1" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="F1" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="H1" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="I1" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="J1" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="K1" s="26" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" s="6" customFormat="1" ht="10.199999999999999" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="15" t="s">
         <v>165</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E2" s="6" t="s">
         <v>166</v>
       </c>
-      <c r="F1" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" s="6" customFormat="1" ht="10.199999999999999" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
-        <v>140</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>139</v>
-      </c>
-      <c r="C2" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="16" t="s">
-        <v>169</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>170</v>
-      </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="27" t="s">
+        <v>141</v>
+      </c>
+      <c r="G2" s="27" t="s">
+        <v>142</v>
+      </c>
+      <c r="H2" s="27" t="s">
+        <v>143</v>
+      </c>
+      <c r="I2" s="27" t="s">
+        <v>144</v>
+      </c>
+      <c r="J2" s="27" t="s">
         <v>145</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="K2" s="27" t="s">
         <v>146</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>150</v>
       </c>
     </row>
   </sheetData>
@@ -3095,7 +3081,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" style="15" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" style="14" customWidth="1"/>
     <col min="2" max="2" width="19.109375" style="2" customWidth="1"/>
     <col min="3" max="3" width="13.109375" style="2" customWidth="1"/>
     <col min="4" max="4" width="14.77734375" style="2" customWidth="1"/>
@@ -3107,7 +3093,7 @@
   <sheetData>
     <row r="1" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>1</v>
@@ -3116,21 +3102,21 @@
         <v>2</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="6" customFormat="1" ht="10.199999999999999" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
-        <v>152</v>
-      </c>
-      <c r="B2" s="15" t="s">
+      <c r="A2" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="B2" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="15" t="s">
         <v>10</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -3162,7 +3148,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.21875" style="17" customWidth="1"/>
+    <col min="1" max="1" width="18.21875" style="16" customWidth="1"/>
     <col min="2" max="3" width="16.5546875" style="2" customWidth="1"/>
     <col min="4" max="4" width="23.88671875" style="2" customWidth="1"/>
     <col min="5" max="16384" width="8.88671875" style="2"/>
@@ -3170,7 +3156,7 @@
   <sheetData>
     <row r="1" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>1</v>
@@ -3179,21 +3165,21 @@
         <v>2</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="6" customFormat="1" ht="10.199999999999999" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
-        <v>153</v>
-      </c>
-      <c r="B2" s="15" t="s">
+      <c r="A2" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="B2" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="15" t="s">
         <v>10</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
   </sheetData>
@@ -3221,7 +3207,7 @@
   <sheetData>
     <row r="1" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>1</v>
@@ -3230,21 +3216,21 @@
         <v>2</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="6" customFormat="1" ht="10.199999999999999" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="B2" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="B2" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="15" t="s">
         <v>10</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -3263,7 +3249,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.44140625" style="17" customWidth="1"/>
+    <col min="1" max="1" width="22.44140625" style="16" customWidth="1"/>
     <col min="2" max="2" width="16" style="2" customWidth="1"/>
     <col min="3" max="3" width="15.88671875" style="2" customWidth="1"/>
     <col min="4" max="4" width="17.6640625" style="2" customWidth="1"/>
@@ -3272,7 +3258,7 @@
   <sheetData>
     <row r="1" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>1</v>
@@ -3281,21 +3267,21 @@
         <v>2</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="6" customFormat="1" ht="10.199999999999999" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="B2" s="15" t="s">
+        <v>140</v>
+      </c>
+      <c r="B2" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="15" t="s">
         <v>10</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>
@@ -3314,7 +3300,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.88671875" style="17" customWidth="1"/>
+    <col min="1" max="1" width="26.88671875" style="16" customWidth="1"/>
     <col min="2" max="3" width="17.77734375" style="2" customWidth="1"/>
     <col min="4" max="4" width="31.109375" style="2" customWidth="1"/>
     <col min="5" max="5" width="17.6640625" style="2" customWidth="1"/>
@@ -3324,7 +3310,7 @@
   <sheetData>
     <row r="1" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>1</v>
@@ -3333,27 +3319,27 @@
         <v>2</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
     </row>
     <row r="2" spans="1:13" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="15" t="s">
-        <v>103</v>
+      <c r="D2" s="14" t="s">
+        <v>101</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
@@ -3398,7 +3384,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.6640625" style="17" customWidth="1"/>
+    <col min="1" max="1" width="25.6640625" style="16" customWidth="1"/>
     <col min="2" max="2" width="18" style="2" customWidth="1"/>
     <col min="3" max="3" width="17.77734375" style="2" customWidth="1"/>
     <col min="4" max="4" width="34.5546875" style="2" customWidth="1"/>
@@ -3409,7 +3395,7 @@
   <sheetData>
     <row r="1" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>1</v>
@@ -3418,27 +3404,27 @@
         <v>2</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="6" customFormat="1" ht="10.199999999999999" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="B2" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="B2" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="15" t="s">
-        <v>102</v>
+      <c r="D2" s="14" t="s">
+        <v>100</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -3475,7 +3461,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.6640625" style="17" customWidth="1"/>
+    <col min="1" max="1" width="25.6640625" style="16" customWidth="1"/>
     <col min="2" max="2" width="24" style="2" customWidth="1"/>
     <col min="3" max="3" width="18.88671875" style="2" customWidth="1"/>
     <col min="4" max="4" width="28.33203125" style="2" customWidth="1"/>
@@ -3485,7 +3471,7 @@
   <sheetData>
     <row r="1" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>1</v>
@@ -3494,27 +3480,27 @@
         <v>2</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
     </row>
     <row r="2" spans="1:13" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="E2" s="17" t="s">
         <v>109</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="E2" s="18" t="s">
-        <v>111</v>
       </c>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
@@ -3534,25 +3520,27 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:U22"/>
+  <dimension ref="A1:V22"/>
   <sheetViews>
-    <sheetView topLeftCell="O1" zoomScale="102" zoomScaleNormal="102" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView topLeftCell="Q1" zoomScale="102" zoomScaleNormal="102" workbookViewId="0">
+      <selection activeCell="U1" activeCellId="5" sqref="Q1 Q1:Q1048576 R1:R1048576 S1:S1048576 T1:T1048576 U1:U1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.6640625" style="7"/>
-    <col min="2" max="13" width="30.6640625" style="2"/>
-    <col min="14" max="14" width="38.6640625" style="2" customWidth="1"/>
-    <col min="15" max="15" width="27.33203125" style="2" customWidth="1"/>
-    <col min="16" max="21" width="30.6640625" style="2"/>
-    <col min="22" max="16384" width="8.88671875" style="2"/>
+    <col min="2" max="3" width="30.6640625" style="2"/>
+    <col min="4" max="4" width="36.109375" style="2" customWidth="1"/>
+    <col min="5" max="14" width="30.6640625" style="2"/>
+    <col min="15" max="15" width="38.6640625" style="2" customWidth="1"/>
+    <col min="16" max="16" width="27.33203125" style="2" customWidth="1"/>
+    <col min="17" max="22" width="30.6640625" style="25"/>
+    <col min="23" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>1</v>
@@ -3561,127 +3549,133 @@
         <v>2</v>
       </c>
       <c r="D1" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="L1" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="M1" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="K1" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="M1" s="5" t="s">
-        <v>158</v>
-      </c>
       <c r="N1" s="5" t="s">
-        <v>172</v>
+        <v>154</v>
       </c>
       <c r="O1" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q1" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="R1" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="S1" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="T1" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="U1" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="V1" s="26" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="U1" s="5" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="2" spans="1:21" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="B2" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>229</v>
+      </c>
+      <c r="E2" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="6" t="s">
+      <c r="F2" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="G2" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="H2" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="I2" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="J2" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="K2" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="L2" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="M2" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="N2" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="M2" s="6" t="s">
+      <c r="O2" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="P2" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q2" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="N2" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="O2" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="P2" s="6" t="s">
+      <c r="R2" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="Q2" s="6" t="s">
+      <c r="S2" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="R2" s="6" t="s">
+      <c r="T2" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="S2" s="6" t="s">
+      <c r="U2" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="T2" s="6" t="s">
+      <c r="V2" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="U2" s="6" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A3" s="19"/>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A3" s="18"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -3696,15 +3690,16 @@
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
-      <c r="P3" s="20"/>
-      <c r="Q3" s="20"/>
-      <c r="R3" s="20"/>
-      <c r="S3" s="20"/>
-      <c r="T3" s="20"/>
-      <c r="U3" s="20"/>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A4" s="19"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="23"/>
+      <c r="R3" s="23"/>
+      <c r="S3" s="23"/>
+      <c r="T3" s="23"/>
+      <c r="U3" s="23"/>
+      <c r="V3" s="23"/>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A4" s="18"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -3720,14 +3715,15 @@
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
-      <c r="Q4" s="1"/>
-      <c r="R4" s="1"/>
-      <c r="S4" s="1"/>
-      <c r="T4" s="1"/>
-      <c r="U4" s="1"/>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A5" s="19"/>
+      <c r="Q4" s="24"/>
+      <c r="R4" s="24"/>
+      <c r="S4" s="24"/>
+      <c r="T4" s="24"/>
+      <c r="U4" s="24"/>
+      <c r="V4" s="24"/>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A5" s="18"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -3743,14 +3739,15 @@
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
-      <c r="Q5" s="1"/>
-      <c r="R5" s="1"/>
-      <c r="S5" s="1"/>
-      <c r="T5" s="1"/>
-      <c r="U5" s="1"/>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A6" s="19"/>
+      <c r="Q5" s="24"/>
+      <c r="R5" s="24"/>
+      <c r="S5" s="24"/>
+      <c r="T5" s="24"/>
+      <c r="U5" s="24"/>
+      <c r="V5" s="24"/>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A6" s="18"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -3766,14 +3763,15 @@
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
-      <c r="Q6" s="1"/>
-      <c r="R6" s="1"/>
-      <c r="S6" s="1"/>
-      <c r="T6" s="1"/>
-      <c r="U6" s="1"/>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A7" s="19"/>
+      <c r="Q6" s="24"/>
+      <c r="R6" s="24"/>
+      <c r="S6" s="24"/>
+      <c r="T6" s="24"/>
+      <c r="U6" s="24"/>
+      <c r="V6" s="24"/>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A7" s="18"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -3789,14 +3787,15 @@
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
-      <c r="Q7" s="1"/>
-      <c r="R7" s="1"/>
-      <c r="S7" s="1"/>
-      <c r="T7" s="1"/>
-      <c r="U7" s="1"/>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A8" s="19"/>
+      <c r="Q7" s="24"/>
+      <c r="R7" s="24"/>
+      <c r="S7" s="24"/>
+      <c r="T7" s="24"/>
+      <c r="U7" s="24"/>
+      <c r="V7" s="24"/>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A8" s="18"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -3812,82 +3811,100 @@
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
-      <c r="Q8" s="1"/>
-      <c r="R8" s="1"/>
-      <c r="S8" s="1"/>
-      <c r="T8" s="1"/>
-      <c r="U8" s="1"/>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="Q8" s="24"/>
+      <c r="R8" s="24"/>
+      <c r="S8" s="24"/>
+      <c r="T8" s="24"/>
+      <c r="U8" s="24"/>
+      <c r="V8" s="24"/>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D16" s="1"/>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B18" s="21"/>
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18" s="19"/>
       <c r="C18" s="1"/>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D18" s="1"/>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D19" s="1"/>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D20" s="1"/>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D21" s="1"/>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error" error="You must select one of the values available in the drop-down list box" sqref="E3:E501" xr:uid="{00000000-0002-0000-0100-000000000000}">
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error" error="You must select one of the values available in the drop-down list box" sqref="F3:F501" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"Software Package,In House Application,Middleware,System,Office System,#reset"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error" error="You must select one of the values available in the drop-down list box" sqref="F3:F501" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error" error="You must select one of the values available in the drop-down list box" sqref="G3:G501" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>"Yes,No,#reset"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3:D1094" xr:uid="{20D91160-34EA-4D0F-9A25-C1CC1FDBAE34}">
+      <formula1>"On-Premises,Cloud: IaaS,Cloud: PaaS,Cloud: SaaS"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Fix State Software Technology WorkSheet
</commit_message>
<xml_diff>
--- a/ITPM - Import Excel Template/MEGA_USR/ITPM Template v4.xlsx
+++ b/ITPM - Import Excel Template/MEGA_USR/ITPM Template v4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MAM\Desktop\ITPM - Import Excel Template\MEGA_USR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F61D862-26C2-4E1F-9849-9612FC65286B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E86B09A-22FE-4DC1-B513-9B0191BA5974}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="961" firstSheet="6" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="961" firstSheet="6" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="_README" sheetId="18" r:id="rId1"/>
@@ -618,7 +618,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="244">
   <si>
     <t>Software Technology</t>
   </si>
@@ -1335,13 +1335,43 @@
   <si>
     <t>809C94A65E1C56CA</t>
   </si>
+  <si>
+    <t>Envisioning Begin Date</t>
+  </si>
+  <si>
+    <t>Envisioning End Date</t>
+  </si>
+  <si>
+    <t>Emerging Begin Date</t>
+  </si>
+  <si>
+    <t>Emerging End Date</t>
+  </si>
+  <si>
+    <t>Confirmed Begin Date</t>
+  </si>
+  <si>
+    <t>Confirmed End Date</t>
+  </si>
+  <si>
+    <t>Obsolete Begin Date</t>
+  </si>
+  <si>
+    <t>Obsolete End Date</t>
+  </si>
+  <si>
+    <t>2D4C3B0C54364275</t>
+  </si>
+  <si>
+    <t>2D4C3B1C543642B5</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy/m/d;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy/m/d;@"/>
   </numFmts>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
@@ -1518,22 +1548,22 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2108,10 +2138,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q12"/>
+  <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView zoomScale="102" zoomScaleNormal="102" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+    <sheetView tabSelected="1" zoomScale="102" zoomScaleNormal="102" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2120,9 +2150,8 @@
     <col min="2" max="4" width="30.6640625" style="2"/>
     <col min="5" max="5" width="27.33203125" style="2" customWidth="1"/>
     <col min="6" max="6" width="30.6640625" style="25"/>
-    <col min="7" max="9" width="30.6640625" style="2"/>
-    <col min="10" max="15" width="30.6640625" style="25"/>
-    <col min="16" max="17" width="30.6640625" style="2"/>
+    <col min="7" max="7" width="30.6640625" style="2"/>
+    <col min="8" max="17" width="30.6640625" style="25"/>
     <col min="18" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
@@ -2148,29 +2177,35 @@
       <c r="G1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="26" t="s">
         <v>7</v>
       </c>
       <c r="J1" s="26" t="s">
-        <v>32</v>
+        <v>234</v>
       </c>
       <c r="K1" s="26" t="s">
-        <v>33</v>
+        <v>235</v>
       </c>
       <c r="L1" s="26" t="s">
-        <v>34</v>
+        <v>236</v>
       </c>
       <c r="M1" s="26" t="s">
-        <v>35</v>
+        <v>237</v>
       </c>
       <c r="N1" s="26" t="s">
-        <v>36</v>
+        <v>238</v>
       </c>
       <c r="O1" s="26" t="s">
-        <v>118</v>
+        <v>239</v>
+      </c>
+      <c r="P1" s="26" t="s">
+        <v>240</v>
+      </c>
+      <c r="Q1" s="26" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="2" spans="1:17" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -2195,10 +2230,10 @@
       <c r="G2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="27" t="s">
         <v>14</v>
       </c>
       <c r="J2" s="27" t="s">
@@ -2219,54 +2254,18 @@
       <c r="O2" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="P2" s="6"/>
-      <c r="Q2" s="6"/>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
+      <c r="P2" s="27" t="s">
+        <v>242</v>
+      </c>
+      <c r="Q2" s="27" t="s">
+        <v>243</v>
+      </c>
     </row>
   </sheetData>
   <dataConsolidate/>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error" error="You must select one of the values available in the drop-down list box" sqref="F13:F501 G3:G12" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error" error="You must select one of the values available in the drop-down list box" sqref="F12:F500 G3:G11" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Expected,Accepted,Prohibited,Unknown,#reset"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2964,7 +2963,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{054DD31E-EE39-4F1E-91F5-CA20AA5F6A1D}">
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="K1" activeCellId="6" sqref="F8 F1:F1048576 G1:G1048576 H1:H1048576 I1:I1048576 J1:J1048576 K1:K1048576"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fix:Wrong CLoud Computing IdAbs
</commit_message>
<xml_diff>
--- a/ITPM - Import Excel Template/MEGA_USR/ITPM Template v4.xlsx
+++ b/ITPM - Import Excel Template/MEGA_USR/ITPM Template v4.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MAM\Desktop\ITPM - Import Excel Template\MEGA_USR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git Store\excel-templates\ITPM - Import Excel Template\MEGA_USR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E86B09A-22FE-4DC1-B513-9B0191BA5974}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75596DE8-62A2-4CA1-BA82-AB1B1796F901}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="961" firstSheet="6" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="961" firstSheet="6" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="_README" sheetId="18" r:id="rId1"/>
@@ -1321,9 +1321,6 @@
     <t>Cloud Computing</t>
   </si>
   <si>
-    <t>=D1:D636Cloud Computing</t>
-  </si>
-  <si>
     <t>A6F59BA55EA97E29</t>
   </si>
   <si>
@@ -1364,6 +1361,9 @@
   </si>
   <si>
     <t>2D4C3B1C543642B5</t>
+  </si>
+  <si>
+    <t>268D381253A01615</t>
   </si>
 </sst>
 </file>
@@ -2140,7 +2140,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="102" zoomScaleNormal="102" workbookViewId="0">
+    <sheetView zoomScale="102" zoomScaleNormal="102" workbookViewId="0">
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
@@ -2184,28 +2184,28 @@
         <v>7</v>
       </c>
       <c r="J1" s="26" t="s">
+        <v>233</v>
+      </c>
+      <c r="K1" s="26" t="s">
         <v>234</v>
       </c>
-      <c r="K1" s="26" t="s">
+      <c r="L1" s="26" t="s">
         <v>235</v>
       </c>
-      <c r="L1" s="26" t="s">
+      <c r="M1" s="26" t="s">
         <v>236</v>
       </c>
-      <c r="M1" s="26" t="s">
+      <c r="N1" s="26" t="s">
         <v>237</v>
       </c>
-      <c r="N1" s="26" t="s">
+      <c r="O1" s="26" t="s">
         <v>238</v>
       </c>
-      <c r="O1" s="26" t="s">
+      <c r="P1" s="26" t="s">
         <v>239</v>
       </c>
-      <c r="P1" s="26" t="s">
+      <c r="Q1" s="26" t="s">
         <v>240</v>
-      </c>
-      <c r="Q1" s="26" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="2" spans="1:17" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -2225,7 +2225,7 @@
         <v>105</v>
       </c>
       <c r="F2" s="27" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G2" s="6" t="s">
         <v>12</v>
@@ -2255,10 +2255,10 @@
         <v>20</v>
       </c>
       <c r="P2" s="27" t="s">
+        <v>241</v>
+      </c>
+      <c r="Q2" s="27" t="s">
         <v>242</v>
-      </c>
-      <c r="Q2" s="27" t="s">
-        <v>243</v>
       </c>
     </row>
   </sheetData>
@@ -2370,7 +2370,7 @@
         <v>68</v>
       </c>
       <c r="J2" s="27" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="K2" s="6" t="s">
         <v>69</v>
@@ -2916,10 +2916,10 @@
         <v>119</v>
       </c>
       <c r="H2" s="27" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="I2" s="27" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -3521,8 +3521,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:V22"/>
   <sheetViews>
-    <sheetView topLeftCell="Q1" zoomScale="102" zoomScaleNormal="102" workbookViewId="0">
-      <selection activeCell="U1" activeCellId="5" sqref="Q1 Q1:Q1048576 R1:R1048576 S1:S1048576 T1:T1048576 U1:U1048576"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="102" zoomScaleNormal="102" workbookViewId="0">
+      <selection activeCell="B2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -3616,7 +3616,7 @@
         <v>10</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>229</v>
+        <v>243</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>38</v>

</xml_diff>

<commit_message>
Owner is not systematically set when importing with Excel Template
</commit_message>
<xml_diff>
--- a/ITPM - Import Excel Template/MEGA_USR/ITPM Template v4.xlsx
+++ b/ITPM - Import Excel Template/MEGA_USR/ITPM Template v4.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git Store\excel-templates\ITPM - Import Excel Template\MEGA_USR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MAM\Desktop\ste\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75596DE8-62A2-4CA1-BA82-AB1B1796F901}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6E2031D-7651-4B15-8C7D-31F2F79A8413}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="961" firstSheet="6" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3522,7 +3522,7 @@
   <dimension ref="A1:V22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="102" zoomScaleNormal="102" workbookViewId="0">
-      <selection activeCell="B2" sqref="A2:XFD2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>

</xml_diff>